<commit_message>
Combined table for vaccines
</commit_message>
<xml_diff>
--- a/app/config/tables/MIFVISIT_CORE/forms/MIFVISIT_CORE/MIFVISIT_CORE.xlsx
+++ b/app/config/tables/MIFVISIT_CORE/forms/MIFVISIT_CORE/MIFVISIT_CORE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8DEAB4-E244-4197-A1DB-B65BEBAD2DCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFD006F-C97E-4BEA-A6E7-0CD518450DF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -945,7 +945,7 @@
     <t>Vac</t>
   </si>
   <si>
-    <t>MIFVAC_MUL</t>
+    <t>MIFVAC</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F91" sqref="F91"/>
     </sheetView>
@@ -3665,7 +3665,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3796,7 +3796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:C1048576"/>
     </sheetView>

</xml_diff>